<commit_message>
before 3.21; feature selection on 135 features done
</commit_message>
<xml_diff>
--- a/prediction_models/experiments/pitched_instrument_regression/feature_selection/featureList.xlsx
+++ b/prediction_models/experiments/pitched_instrument_regression/feature_selection/featureList.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caspia/Desktop/Github/FBA_code_2019/src/prediction_models/experiments/pitched_instrument_regression/feature_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590A3609-CA07-7340-A944-35D3E9A0A170}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC79EBE-994C-AE42-BB90-6E938238734D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="480" windowWidth="21800" windowHeight="16160" xr2:uid="{EDC135E0-EA88-8D45-85C0-D72C03D30815}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="2" xr2:uid="{EDC135E0-EA88-8D45-85C0-D72C03D30815}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="note seg" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="106">
   <si>
     <t>std features</t>
   </si>
@@ -285,6 +287,81 @@
   </si>
   <si>
     <t>rhythmic-IOI</t>
+  </si>
+  <si>
+    <t>PCA-1</t>
+  </si>
+  <si>
+    <t>PCA-2</t>
+  </si>
+  <si>
+    <t>PCA-3</t>
+  </si>
+  <si>
+    <t>sight-reading</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>dtw-related &amp; note deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>note length ratio (rhythmic)</t>
+  </si>
+  <si>
+    <t>spectral (MFCCs)</t>
+  </si>
+  <si>
+    <t>PCA-4</t>
+  </si>
+  <si>
+    <t>PCA-5</t>
+  </si>
+  <si>
+    <t>std of std (std features)</t>
+  </si>
+  <si>
+    <t>note length ratio features: all deviations except one</t>
+  </si>
+  <si>
+    <t>dtw cost and jump features</t>
+  </si>
+  <si>
+    <t>correlation within spectral features</t>
+  </si>
+  <si>
+    <t>spectral features and mean of note length ratio (speed related)</t>
+  </si>
+  <si>
+    <t>close to PCA-1 of sight-reading</t>
+  </si>
+  <si>
+    <t>DTW-related features: 105, 114:117</t>
+  </si>
+  <si>
+    <t>note length ratio (mean): 118, 120, 125, 127, 129, 131, 133</t>
+  </si>
+  <si>
+    <t>note length ratio (std): 119, 121, 126, 128, 130, 132, 134</t>
+  </si>
+  <si>
+    <t>std features?</t>
+  </si>
+  <si>
+    <t>PlayingNotes100CntsHist</t>
+  </si>
+  <si>
+    <t>correct number of notes</t>
+  </si>
+  <si>
+    <t>number of notes returned by notesegmentation()</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
   </si>
 </sst>
 </file>
@@ -315,7 +392,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +435,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -371,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,6 +491,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -403,17 +515,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -731,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95F1AD7-3167-D948-BE34-BAACF79AC7EE}">
   <dimension ref="A1:R136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,17 +891,17 @@
       <c r="C2" s="6"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="O2" s="16"/>
+      <c r="I2" s="10"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -804,13 +911,13 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="15"/>
-      <c r="O3" s="16"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="10"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -820,13 +927,13 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="15"/>
-      <c r="O4" s="16"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="10"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -836,13 +943,13 @@
       <c r="C5" s="6"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="J5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="H5" s="22"/>
+      <c r="J5" s="11"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -852,13 +959,13 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="15"/>
-      <c r="O6" s="16"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="10"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -868,11 +975,11 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="15"/>
-      <c r="O7" s="16"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="10"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -882,11 +989,11 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="15"/>
-      <c r="O8" s="16"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="10"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -896,11 +1003,11 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="15"/>
-      <c r="O9" s="16"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="10"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -910,11 +1017,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="15"/>
-      <c r="O10" s="16"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="10"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -924,11 +1031,11 @@
       <c r="C11" s="1"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="15"/>
-      <c r="O11" s="16"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="10"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -938,11 +1045,11 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="15"/>
-      <c r="O12" s="16"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="10"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -952,11 +1059,11 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="15"/>
-      <c r="O13" s="16"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="10"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -966,11 +1073,11 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="15"/>
-      <c r="O14" s="16"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="10"/>
+      <c r="O14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -980,11 +1087,11 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="15"/>
-      <c r="O15" s="16"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="10"/>
+      <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -994,11 +1101,11 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="15"/>
-      <c r="O16" s="16"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="10"/>
+      <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1008,11 +1115,11 @@
       <c r="C17" s="6"/>
       <c r="D17" s="1"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="15"/>
-      <c r="O17" s="16"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="10"/>
+      <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1022,11 +1129,11 @@
       <c r="C18" s="1"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="15"/>
-      <c r="O18" s="16"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="10"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1036,16 +1143,16 @@
       <c r="C19" s="6"/>
       <c r="D19" s="1"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="12"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="15"/>
+      <c r="I19" s="10"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1055,14 +1162,14 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="12"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="15"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="15"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="10"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1072,14 +1179,14 @@
       <c r="C21" s="6"/>
       <c r="D21" s="1"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="12"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="15"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="15"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="10"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1089,14 +1196,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="12"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="J22" s="16"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="15"/>
+      <c r="H22" s="22"/>
+      <c r="J22" s="11"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="10"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1106,14 +1213,14 @@
       <c r="C23" s="6"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11" t="s">
+      <c r="F23" s="20"/>
+      <c r="G23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="15"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="15"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="10"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1123,12 +1230,12 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="15"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="15"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="10"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1138,12 +1245,12 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="15"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="15"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="10"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1153,12 +1260,12 @@
       <c r="C26" s="6"/>
       <c r="D26" s="1"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="15"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="15"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="10"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1168,12 +1275,12 @@
       <c r="C27" s="1"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="15"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="15"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="10"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="10"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1183,12 +1290,12 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="15"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="15"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="10"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="10"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1198,12 +1305,12 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="15"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="15"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="10"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1213,12 +1320,12 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="15"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="15"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="10"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1228,12 +1335,12 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="15"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="15"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="10"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1243,12 +1350,12 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="15"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="15"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="10"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1258,12 +1365,12 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="15"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="15"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="10"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -1273,12 +1380,12 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="15"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="15"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="10"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -1288,12 +1395,12 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="15"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="15"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="10"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="10"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -1303,16 +1410,16 @@
       <c r="C36" s="6"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="12"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H36" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I36" s="15"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="15"/>
+      <c r="I36" s="10"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1322,14 +1429,14 @@
       <c r="C37" s="1"/>
       <c r="D37" s="8"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="12"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="15"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="15"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="10"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="10"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -1339,14 +1446,14 @@
       <c r="C38" s="6"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="12"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="15"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="15"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="10"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="10"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -1356,14 +1463,14 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="12"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="11"/>
-      <c r="J39" s="16"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="15"/>
+      <c r="H39" s="22"/>
+      <c r="J39" s="11"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="10"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -1373,14 +1480,14 @@
       <c r="C40" s="6"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="11" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="15"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="15"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="10"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="10"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -1390,12 +1497,12 @@
       <c r="C41" s="6"/>
       <c r="D41" s="1"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="15"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="15"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="10"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="10"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -1405,12 +1512,12 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="15"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="15"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="10"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="10"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -1420,12 +1527,12 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="15"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="15"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="10"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="10"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1435,12 +1542,12 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="15"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="15"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="10"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="10"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -1450,12 +1557,12 @@
       <c r="C45" s="6"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="15"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="15"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="10"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="10"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -1465,12 +1572,12 @@
       <c r="C46" s="6"/>
       <c r="D46" s="8"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="15"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="15"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="10"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="10"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -1480,12 +1587,12 @@
       <c r="C47" s="6"/>
       <c r="D47" s="1"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="15"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="15"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="10"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="10"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -1495,12 +1602,12 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="15"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="15"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="10"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="10"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -1510,12 +1617,12 @@
       <c r="C49" s="6"/>
       <c r="D49" s="1"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="15"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="15"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="10"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="10"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -1525,12 +1632,12 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="15"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="15"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="10"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="10"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -1540,12 +1647,12 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="15"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="15"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="10"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="10"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -1555,12 +1662,12 @@
       <c r="C52" s="6"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="15"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="15"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="10"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="10"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -1570,15 +1677,15 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="12"/>
+      <c r="F53" s="20"/>
       <c r="G53" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="P53" s="16"/>
+      <c r="I53" s="10"/>
+      <c r="P53" s="11"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -1588,13 +1695,13 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="12"/>
+      <c r="F54" s="20"/>
       <c r="G54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H54" s="11"/>
-      <c r="I54" s="15"/>
-      <c r="P54" s="16"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="10"/>
+      <c r="P54" s="11"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -1604,13 +1711,13 @@
       <c r="C55" s="6"/>
       <c r="D55" s="1"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="12"/>
+      <c r="F55" s="20"/>
       <c r="G55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="15"/>
-      <c r="P55" s="16"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="10"/>
+      <c r="P55" s="11"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -1620,13 +1727,13 @@
       <c r="C56" s="6"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="12"/>
+      <c r="F56" s="20"/>
       <c r="G56" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H56" s="11"/>
-      <c r="J56" s="16"/>
-      <c r="P56" s="16"/>
+      <c r="H56" s="22"/>
+      <c r="J56" s="11"/>
+      <c r="P56" s="11"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -1636,13 +1743,13 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="9"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="11" t="s">
+      <c r="F57" s="20"/>
+      <c r="G57" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="15"/>
-      <c r="P57" s="16"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="10"/>
+      <c r="P57" s="11"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -1652,11 +1759,11 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="15"/>
-      <c r="P58" s="16"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="10"/>
+      <c r="P58" s="11"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -1666,11 +1773,11 @@
       <c r="C59" s="1"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="15"/>
-      <c r="P59" s="16"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="10"/>
+      <c r="P59" s="11"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -1680,11 +1787,11 @@
       <c r="C60" s="6"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="15"/>
-      <c r="P60" s="16"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="10"/>
+      <c r="P60" s="11"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -1694,11 +1801,11 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="15"/>
-      <c r="P61" s="16"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="10"/>
+      <c r="P61" s="11"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -1708,11 +1815,11 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="15"/>
-      <c r="P62" s="16"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="10"/>
+      <c r="P62" s="11"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -1722,11 +1829,11 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="9"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="15"/>
-      <c r="P63" s="16"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="10"/>
+      <c r="P63" s="11"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -1736,11 +1843,11 @@
       <c r="C64" s="6"/>
       <c r="D64" s="8"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="15"/>
-      <c r="P64" s="16"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="10"/>
+      <c r="P64" s="11"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -1750,11 +1857,11 @@
       <c r="C65" s="6"/>
       <c r="D65" s="1"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="15"/>
-      <c r="P65" s="16"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="10"/>
+      <c r="P65" s="11"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -1764,11 +1871,11 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="15"/>
-      <c r="P66" s="16"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="10"/>
+      <c r="P66" s="11"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -1778,11 +1885,11 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="15"/>
-      <c r="P67" s="16"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="10"/>
+      <c r="P67" s="11"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -1792,11 +1899,11 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="15"/>
-      <c r="P68" s="16"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
+      <c r="I68" s="10"/>
+      <c r="P68" s="11"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -1806,11 +1913,11 @@
       <c r="C69" s="6"/>
       <c r="D69" s="1"/>
       <c r="E69" s="9"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="15"/>
-      <c r="P69" s="16"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="10"/>
+      <c r="P69" s="11"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -1820,16 +1927,16 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="9"/>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H70" s="13" t="s">
+      <c r="H70" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O70" s="16"/>
+      <c r="O70" s="11"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -1839,12 +1946,12 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="9"/>
-      <c r="F71" s="12"/>
+      <c r="F71" s="20"/>
       <c r="G71" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H71" s="14"/>
-      <c r="P71" s="16"/>
+      <c r="H71" s="24"/>
+      <c r="P71" s="11"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -1854,12 +1961,12 @@
       <c r="C72" s="6"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="12"/>
+      <c r="F72" s="20"/>
       <c r="G72" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H72" s="14"/>
-      <c r="Q72" s="16"/>
+      <c r="H72" s="24"/>
+      <c r="Q72" s="11"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
@@ -1869,12 +1976,12 @@
       <c r="C73" s="1"/>
       <c r="D73" s="8"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="12"/>
+      <c r="F73" s="20"/>
       <c r="G73" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H73" s="14"/>
-      <c r="R73" s="16"/>
+      <c r="H73" s="24"/>
+      <c r="R73" s="11"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -1884,12 +1991,12 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="12"/>
+      <c r="F74" s="20"/>
       <c r="G74" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H74" s="14"/>
-      <c r="O74" s="16"/>
+      <c r="H74" s="24"/>
+      <c r="O74" s="11"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -1899,12 +2006,12 @@
       <c r="C75" s="6"/>
       <c r="D75" s="1"/>
       <c r="E75" s="9"/>
-      <c r="F75" s="12"/>
+      <c r="F75" s="20"/>
       <c r="G75" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="14"/>
-      <c r="P75" s="16"/>
+      <c r="H75" s="24"/>
+      <c r="P75" s="11"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -1914,12 +2021,12 @@
       <c r="C76" s="6"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="12"/>
+      <c r="F76" s="20"/>
       <c r="G76" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H76" s="14"/>
-      <c r="Q76" s="16"/>
+      <c r="H76" s="24"/>
+      <c r="Q76" s="11"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -1929,12 +2036,12 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="12"/>
+      <c r="F77" s="20"/>
       <c r="G77" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H77" s="14"/>
-      <c r="R77" s="16"/>
+      <c r="H77" s="24"/>
+      <c r="R77" s="11"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -1944,12 +2051,12 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="12"/>
+      <c r="F78" s="20"/>
       <c r="G78" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H78" s="14"/>
-      <c r="O78" s="16"/>
+      <c r="H78" s="24"/>
+      <c r="O78" s="11"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -1959,12 +2066,12 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="12"/>
+      <c r="F79" s="20"/>
       <c r="G79" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H79" s="14"/>
-      <c r="P79" s="16"/>
+      <c r="H79" s="24"/>
+      <c r="P79" s="11"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -1974,12 +2081,12 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="12"/>
+      <c r="F80" s="20"/>
       <c r="G80" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H80" s="14"/>
-      <c r="Q80" s="16"/>
+      <c r="H80" s="24"/>
+      <c r="Q80" s="11"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
@@ -1989,12 +2096,12 @@
       <c r="C81" s="1"/>
       <c r="D81" s="8"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="12"/>
+      <c r="F81" s="20"/>
       <c r="G81" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H81" s="14"/>
-      <c r="R81" s="16"/>
+      <c r="H81" s="24"/>
+      <c r="R81" s="11"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
@@ -2004,12 +2111,12 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="9"/>
-      <c r="F82" s="12"/>
+      <c r="F82" s="20"/>
       <c r="G82" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H82" s="14"/>
-      <c r="O82" s="16"/>
+      <c r="H82" s="24"/>
+      <c r="O82" s="11"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -2019,12 +2126,12 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="9"/>
-      <c r="F83" s="12"/>
+      <c r="F83" s="20"/>
       <c r="G83" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H83" s="14"/>
-      <c r="P83" s="16"/>
+      <c r="H83" s="24"/>
+      <c r="P83" s="11"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -2034,12 +2141,12 @@
       <c r="C84" s="6"/>
       <c r="D84" s="1"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="12"/>
+      <c r="F84" s="20"/>
       <c r="G84" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H84" s="14"/>
-      <c r="Q84" s="16"/>
+      <c r="H84" s="24"/>
+      <c r="Q84" s="11"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2049,12 +2156,12 @@
       <c r="C85" s="6"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="12"/>
+      <c r="F85" s="20"/>
       <c r="G85" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H85" s="14"/>
-      <c r="R85" s="16"/>
+      <c r="H85" s="24"/>
+      <c r="R85" s="11"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
@@ -2064,7 +2171,7 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="12"/>
+      <c r="F86" s="20"/>
       <c r="G86" s="3" t="s">
         <v>50</v>
       </c>
@@ -2078,12 +2185,13 @@
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="11" t="s">
+      <c r="F87" s="20"/>
+      <c r="G87" s="22" t="s">
         <v>51</v>
       </c>
       <c r="H87" s="2"/>
-      <c r="L87" s="17"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="12"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
@@ -2093,10 +2201,11 @@
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="11"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="22"/>
       <c r="H88" s="2"/>
-      <c r="L88" s="17"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="12"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -2106,10 +2215,11 @@
       <c r="C89" s="6"/>
       <c r="D89" s="8"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="11"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="22"/>
       <c r="H89" s="2"/>
-      <c r="L89" s="17"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="12"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -2119,10 +2229,11 @@
       <c r="C90" s="6"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="11"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="22"/>
       <c r="H90" s="2"/>
-      <c r="L90" s="17"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="12"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -2132,10 +2243,11 @@
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="9"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="11"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="22"/>
       <c r="H91" s="2"/>
-      <c r="L91" s="17"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="12"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -2145,10 +2257,11 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="11"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="22"/>
       <c r="H92" s="2"/>
-      <c r="L92" s="17"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="12"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -2158,10 +2271,11 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="11"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="22"/>
       <c r="H93" s="2"/>
-      <c r="L93" s="17"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="12"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -2171,7 +2285,7 @@
       <c r="C94" s="6"/>
       <c r="D94" s="1"/>
       <c r="E94" s="9"/>
-      <c r="F94" s="12" t="s">
+      <c r="F94" s="20" t="s">
         <v>2</v>
       </c>
       <c r="G94" s="4" t="s">
@@ -2187,13 +2301,13 @@
       <c r="C95" s="6"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="F95" s="12"/>
+      <c r="F95" s="20"/>
       <c r="G95" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H95" s="2"/>
-      <c r="K95" s="16"/>
-      <c r="O95" s="16"/>
+      <c r="K95" s="11"/>
+      <c r="O95" s="11"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -2203,13 +2317,13 @@
       <c r="C96" s="6"/>
       <c r="D96" s="1"/>
       <c r="E96" s="9"/>
-      <c r="F96" s="12"/>
+      <c r="F96" s="20"/>
       <c r="G96" s="3" t="s">
         <v>55</v>
       </c>
       <c r="H96" s="2"/>
-      <c r="K96" s="16"/>
-      <c r="P96" s="16"/>
+      <c r="K96" s="11"/>
+      <c r="P96" s="11"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
@@ -2219,13 +2333,13 @@
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="9"/>
-      <c r="F97" s="12"/>
+      <c r="F97" s="20"/>
       <c r="G97" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H97" s="2"/>
-      <c r="K97" s="16"/>
-      <c r="Q97" s="16"/>
+      <c r="K97" s="11"/>
+      <c r="Q97" s="11"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
@@ -2235,13 +2349,13 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-      <c r="F98" s="12"/>
+      <c r="F98" s="20"/>
       <c r="G98" s="3" t="s">
         <v>57</v>
       </c>
       <c r="H98" s="2"/>
-      <c r="K98" s="16"/>
-      <c r="R98" s="16"/>
+      <c r="K98" s="11"/>
+      <c r="R98" s="11"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
@@ -2251,13 +2365,13 @@
       <c r="C99" s="1"/>
       <c r="D99" s="8"/>
       <c r="E99" s="9"/>
-      <c r="F99" s="12"/>
+      <c r="F99" s="20"/>
       <c r="G99" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H99" s="2"/>
-      <c r="K99" s="16"/>
-      <c r="O99" s="16"/>
+      <c r="K99" s="11"/>
+      <c r="O99" s="11"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
@@ -2267,13 +2381,13 @@
       <c r="C100" s="6"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="F100" s="12"/>
+      <c r="F100" s="20"/>
       <c r="G100" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H100" s="2"/>
-      <c r="K100" s="16"/>
-      <c r="P100" s="16"/>
+      <c r="K100" s="11"/>
+      <c r="P100" s="11"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -2283,13 +2397,13 @@
       <c r="C101" s="6"/>
       <c r="D101" s="8"/>
       <c r="E101" s="9"/>
-      <c r="F101" s="12"/>
+      <c r="F101" s="20"/>
       <c r="G101" s="3" t="s">
         <v>60</v>
       </c>
       <c r="H101" s="2"/>
-      <c r="K101" s="16"/>
-      <c r="Q101" s="16"/>
+      <c r="K101" s="11"/>
+      <c r="Q101" s="11"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -2299,13 +2413,13 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="12"/>
+      <c r="F102" s="20"/>
       <c r="G102" s="3" t="s">
         <v>61</v>
       </c>
       <c r="H102" s="2"/>
-      <c r="K102" s="16"/>
-      <c r="R102" s="16"/>
+      <c r="K102" s="11"/>
+      <c r="R102" s="11"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -2315,13 +2429,13 @@
       <c r="C103" s="6"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="12"/>
+      <c r="F103" s="20"/>
       <c r="G103" s="3" t="s">
         <v>62</v>
       </c>
       <c r="H103" s="2"/>
-      <c r="K103" s="16"/>
-      <c r="O103" s="16"/>
+      <c r="K103" s="11"/>
+      <c r="O103" s="11"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -2331,13 +2445,13 @@
       <c r="C104" s="6"/>
       <c r="D104" s="1"/>
       <c r="E104" s="9"/>
-      <c r="F104" s="12"/>
+      <c r="F104" s="20"/>
       <c r="G104" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H104" s="2"/>
-      <c r="K104" s="16"/>
-      <c r="P104" s="16"/>
+      <c r="K104" s="11"/>
+      <c r="P104" s="11"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -2347,13 +2461,13 @@
       <c r="C105" s="6"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="12"/>
+      <c r="F105" s="20"/>
       <c r="G105" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H105" s="2"/>
-      <c r="K105" s="16"/>
-      <c r="Q105" s="16"/>
+      <c r="K105" s="11"/>
+      <c r="Q105" s="11"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
@@ -2363,13 +2477,13 @@
       <c r="C106" s="6"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" s="12"/>
+      <c r="F106" s="20"/>
       <c r="G106" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H106" s="2"/>
-      <c r="K106" s="16"/>
-      <c r="R106" s="16"/>
+      <c r="K106" s="11"/>
+      <c r="R106" s="11"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
@@ -2379,12 +2493,12 @@
       <c r="C107" s="6"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="12"/>
+      <c r="F107" s="20"/>
       <c r="G107" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H107" s="2"/>
-      <c r="N107" s="16"/>
+      <c r="N107" s="11"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -2394,12 +2508,12 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="12"/>
+      <c r="F108" s="20"/>
       <c r="G108" s="3" t="s">
         <v>67</v>
       </c>
       <c r="H108" s="2"/>
-      <c r="N108" s="16"/>
+      <c r="N108" s="11"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -2409,13 +2523,13 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="9"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="11" t="s">
+      <c r="F109" s="20"/>
+      <c r="G109" s="22" t="s">
         <v>68</v>
       </c>
       <c r="H109" s="2"/>
-      <c r="L109" s="18"/>
-      <c r="M109" s="16"/>
+      <c r="L109" s="13"/>
+      <c r="M109" s="11"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -2425,11 +2539,11 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="11"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="22"/>
       <c r="H110" s="2"/>
-      <c r="L110" s="18"/>
-      <c r="M110" s="16"/>
+      <c r="L110" s="13"/>
+      <c r="M110" s="11"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -2439,11 +2553,11 @@
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="9"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="11"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="22"/>
       <c r="H111" s="2"/>
-      <c r="L111" s="18"/>
-      <c r="M111" s="16"/>
+      <c r="L111" s="13"/>
+      <c r="M111" s="11"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -2453,11 +2567,11 @@
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="9"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="11"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="22"/>
       <c r="H112" s="2"/>
-      <c r="L112" s="18"/>
-      <c r="M112" s="16"/>
+      <c r="L112" s="13"/>
+      <c r="M112" s="11"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -2467,11 +2581,11 @@
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
-      <c r="F113" s="12"/>
-      <c r="G113" s="11"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="22"/>
       <c r="H113" s="2"/>
-      <c r="L113" s="18"/>
-      <c r="M113" s="16"/>
+      <c r="L113" s="13"/>
+      <c r="M113" s="11"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -2481,11 +2595,11 @@
       <c r="C114" s="6"/>
       <c r="D114" s="1"/>
       <c r="E114" s="9"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="11"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="22"/>
       <c r="H114" s="2"/>
-      <c r="L114" s="18"/>
-      <c r="M114" s="16"/>
+      <c r="L114" s="13"/>
+      <c r="M114" s="11"/>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -2495,15 +2609,15 @@
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="9"/>
-      <c r="F115" s="12"/>
+      <c r="F115" s="20"/>
       <c r="G115" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L115" s="16"/>
-      <c r="M115" s="18"/>
+      <c r="L115" s="11"/>
+      <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -2513,14 +2627,14 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
-      <c r="F116" s="12" t="s">
+      <c r="F116" s="20" t="s">
         <v>3</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H116" s="2"/>
-      <c r="N116" s="16"/>
+      <c r="N116" s="11"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
@@ -2530,12 +2644,12 @@
       <c r="C117" s="6"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="12"/>
+      <c r="F117" s="20"/>
       <c r="G117" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="2"/>
-      <c r="N117" s="16"/>
+      <c r="N117" s="11"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
@@ -2545,12 +2659,12 @@
       <c r="C118" s="7"/>
       <c r="D118" s="1"/>
       <c r="E118" s="9"/>
-      <c r="F118" s="12"/>
+      <c r="F118" s="20"/>
       <c r="G118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H118" s="2"/>
-      <c r="N118" s="16"/>
+      <c r="N118" s="11"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
@@ -2560,12 +2674,12 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="9"/>
-      <c r="F119" s="12"/>
+      <c r="F119" s="20"/>
       <c r="G119" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H119" s="2"/>
-      <c r="N119" s="16"/>
+      <c r="N119" s="11"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
@@ -2575,17 +2689,17 @@
       <c r="C120" s="6"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="12" t="s">
+      <c r="F120" s="20" t="s">
         <v>8</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H120" s="10" t="s">
+      <c r="H120" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L120" s="16"/>
-      <c r="O120" s="16"/>
+      <c r="L120" s="11"/>
+      <c r="O120" s="11"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -2595,13 +2709,13 @@
       <c r="C121" s="6"/>
       <c r="D121" s="8"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="12"/>
+      <c r="F121" s="20"/>
       <c r="G121" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H121" s="11"/>
-      <c r="L121" s="16"/>
-      <c r="P121" s="16"/>
+      <c r="H121" s="22"/>
+      <c r="L121" s="11"/>
+      <c r="P121" s="11"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
@@ -2611,14 +2725,14 @@
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
-      <c r="F122" s="12"/>
+      <c r="F122" s="20"/>
       <c r="G122" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H122" s="11"/>
-      <c r="L122" s="16"/>
-      <c r="O122" s="16"/>
-      <c r="Q122" s="18"/>
+      <c r="H122" s="22"/>
+      <c r="L122" s="11"/>
+      <c r="O122" s="11"/>
+      <c r="Q122" s="13"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
@@ -2628,14 +2742,14 @@
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="12"/>
+      <c r="F123" s="20"/>
       <c r="G123" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H123" s="11"/>
-      <c r="L123" s="16"/>
-      <c r="P123" s="16"/>
-      <c r="R123" s="18"/>
+      <c r="H123" s="22"/>
+      <c r="L123" s="11"/>
+      <c r="P123" s="11"/>
+      <c r="R123" s="13"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
@@ -2645,13 +2759,13 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="9"/>
-      <c r="F124" s="12"/>
+      <c r="F124" s="20"/>
       <c r="G124" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H124" s="11"/>
-      <c r="L124" s="16"/>
-      <c r="O124" s="16"/>
+      <c r="H124" s="22"/>
+      <c r="L124" s="11"/>
+      <c r="O124" s="11"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
@@ -2661,13 +2775,13 @@
       <c r="C125" s="6"/>
       <c r="D125" s="1"/>
       <c r="E125" s="9"/>
-      <c r="F125" s="12"/>
+      <c r="F125" s="20"/>
       <c r="G125" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H125" s="11"/>
-      <c r="L125" s="16"/>
-      <c r="P125" s="16"/>
+      <c r="H125" s="22"/>
+      <c r="L125" s="11"/>
+      <c r="P125" s="11"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
@@ -2677,14 +2791,14 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="9"/>
-      <c r="F126" s="12"/>
+      <c r="F126" s="20"/>
       <c r="G126" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H126" s="11"/>
-      <c r="L126" s="16"/>
-      <c r="M126" s="18"/>
-      <c r="Q126" s="18"/>
+      <c r="H126" s="22"/>
+      <c r="L126" s="11"/>
+      <c r="M126" s="13"/>
+      <c r="Q126" s="13"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
@@ -2694,17 +2808,17 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="9"/>
-      <c r="F127" s="12" t="s">
+      <c r="F127" s="20" t="s">
         <v>17</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H127" s="10" t="s">
+      <c r="H127" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L127" s="16"/>
-      <c r="O127" s="16"/>
+      <c r="L127" s="11"/>
+      <c r="O127" s="11"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
@@ -2714,13 +2828,13 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="7"/>
-      <c r="F128" s="12"/>
+      <c r="F128" s="20"/>
       <c r="G128" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H128" s="11"/>
-      <c r="L128" s="16"/>
-      <c r="P128" s="16"/>
+      <c r="H128" s="22"/>
+      <c r="L128" s="11"/>
+      <c r="P128" s="11"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
@@ -2730,13 +2844,13 @@
       <c r="C129" s="6"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="12"/>
+      <c r="F129" s="20"/>
       <c r="G129" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H129" s="11"/>
-      <c r="L129" s="16"/>
-      <c r="O129" s="16"/>
+      <c r="H129" s="22"/>
+      <c r="L129" s="11"/>
+      <c r="O129" s="11"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
@@ -2746,13 +2860,13 @@
       <c r="C130" s="7"/>
       <c r="D130" s="1"/>
       <c r="E130" s="9"/>
-      <c r="F130" s="12"/>
+      <c r="F130" s="20"/>
       <c r="G130" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H130" s="11"/>
-      <c r="L130" s="16"/>
-      <c r="P130" s="16"/>
+      <c r="H130" s="22"/>
+      <c r="L130" s="11"/>
+      <c r="P130" s="11"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
@@ -2762,13 +2876,13 @@
       <c r="C131" s="6"/>
       <c r="D131" s="1"/>
       <c r="E131" s="9"/>
-      <c r="F131" s="12"/>
+      <c r="F131" s="20"/>
       <c r="G131" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H131" s="11"/>
-      <c r="L131" s="16"/>
-      <c r="O131" s="16"/>
+      <c r="H131" s="22"/>
+      <c r="L131" s="11"/>
+      <c r="O131" s="11"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -2778,13 +2892,13 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="12"/>
+      <c r="F132" s="20"/>
       <c r="G132" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H132" s="11"/>
-      <c r="L132" s="16"/>
-      <c r="P132" s="16"/>
+      <c r="H132" s="22"/>
+      <c r="L132" s="11"/>
+      <c r="P132" s="11"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
@@ -2794,17 +2908,17 @@
       <c r="C133" s="6"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="12" t="s">
+      <c r="F133" s="20" t="s">
         <v>19</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H133" s="10" t="s">
+      <c r="H133" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="L133" s="16"/>
-      <c r="O133" s="16"/>
+      <c r="L133" s="11"/>
+      <c r="O133" s="11"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
@@ -2814,13 +2928,13 @@
       <c r="C134" s="6"/>
       <c r="D134" s="1"/>
       <c r="E134" s="9"/>
-      <c r="F134" s="12"/>
+      <c r="F134" s="20"/>
       <c r="G134" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H134" s="11"/>
-      <c r="L134" s="16"/>
-      <c r="P134" s="16"/>
+      <c r="H134" s="22"/>
+      <c r="L134" s="11"/>
+      <c r="P134" s="11"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -2830,17 +2944,17 @@
       <c r="C135" s="1"/>
       <c r="D135" s="8"/>
       <c r="E135" s="9"/>
-      <c r="F135" s="12" t="s">
+      <c r="F135" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H135" s="10" t="s">
+      <c r="H135" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L135" s="16"/>
-      <c r="O135" s="16"/>
+      <c r="L135" s="11"/>
+      <c r="O135" s="11"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
@@ -2850,27 +2964,16 @@
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="9"/>
-      <c r="F136" s="12"/>
+      <c r="F136" s="20"/>
       <c r="G136" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H136" s="10"/>
-      <c r="L136" s="16"/>
-      <c r="P136" s="16"/>
+      <c r="H136" s="21"/>
+      <c r="L136" s="11"/>
+      <c r="P136" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F127:F132"/>
-    <mergeCell ref="H127:H132"/>
-    <mergeCell ref="F133:F134"/>
-    <mergeCell ref="H133:H134"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="H135:H136"/>
-    <mergeCell ref="F2:F69"/>
-    <mergeCell ref="F70:F93"/>
-    <mergeCell ref="F94:F115"/>
-    <mergeCell ref="F116:F119"/>
-    <mergeCell ref="F120:F126"/>
     <mergeCell ref="H120:H126"/>
     <mergeCell ref="H2:H18"/>
     <mergeCell ref="G6:G18"/>
@@ -2883,7 +2986,1901 @@
     <mergeCell ref="G57:G69"/>
     <mergeCell ref="G87:G93"/>
     <mergeCell ref="H70:H85"/>
+    <mergeCell ref="F2:F69"/>
+    <mergeCell ref="F70:F93"/>
+    <mergeCell ref="F94:F115"/>
+    <mergeCell ref="F116:F119"/>
+    <mergeCell ref="F120:F126"/>
+    <mergeCell ref="F127:F132"/>
+    <mergeCell ref="H127:H132"/>
+    <mergeCell ref="F133:F134"/>
+    <mergeCell ref="H133:H134"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="H135:H136"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDD05E0-C001-6B4F-B662-787EB5020951}">
+  <dimension ref="A1:N152"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="G4" s="11"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="F5" s="17"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="G6" s="11"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="I7" s="18"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="G10" s="11"/>
+      <c r="I10" s="18"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="G11" s="11"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="G12" s="11"/>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="G33" s="11"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="G34" s="11"/>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="G36" s="11"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37" s="16"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="22"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="L39" s="16"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="G40" s="11"/>
+      <c r="L40" s="16"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="G41" s="11"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="16"/>
+      <c r="J57" s="19"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="J58" s="19"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" s="20"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" s="20"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" s="20"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" s="20"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" s="20"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" s="20"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" s="20"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" s="20"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="I69" s="18"/>
+      <c r="M69" s="10"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" s="20"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+    </row>
+    <row r="71" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" s="14"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72" s="20"/>
+      <c r="C72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="N72" s="18"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="E73" s="16"/>
+      <c r="N73" s="18"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74" s="20"/>
+      <c r="C74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="24"/>
+      <c r="N74" s="18"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75" s="24"/>
+      <c r="G75" s="11"/>
+      <c r="L75" s="16"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" s="24"/>
+      <c r="N76" s="18"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" s="20"/>
+      <c r="C77" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77" s="24"/>
+      <c r="N77" s="18"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" s="24"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79" s="20"/>
+      <c r="C79" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D79" s="24"/>
+      <c r="E79" s="14"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="C80" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="24"/>
+      <c r="E80" s="15"/>
+      <c r="M80" s="10"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81" s="20"/>
+      <c r="C81" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="24"/>
+      <c r="E81" s="15"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82" s="20"/>
+      <c r="C82" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="24"/>
+      <c r="E82" s="15"/>
+      <c r="M82" s="10"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83" s="20"/>
+      <c r="C83" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="24"/>
+      <c r="E83" s="15"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84" s="20"/>
+      <c r="C84" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" s="24"/>
+      <c r="E84" s="15"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85" s="20"/>
+      <c r="C85" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" s="24"/>
+      <c r="E85" s="15"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86" s="20"/>
+      <c r="C86" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D86" s="24"/>
+      <c r="E86" s="15"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87" s="20"/>
+      <c r="C87" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="24"/>
+      <c r="E87" s="15"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88" s="20"/>
+      <c r="C88" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D88" s="24"/>
+      <c r="E88" s="15"/>
+      <c r="N88" s="18"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89" s="20"/>
+      <c r="C89" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90" s="20"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="K90" s="12"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91" s="20"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92" s="20"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93" s="20"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="J93" s="19"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94" s="20"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D95" s="15"/>
+      <c r="K95" s="12"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96" s="20"/>
+      <c r="C96" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" s="15"/>
+      <c r="K96" s="12"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97" s="20"/>
+      <c r="C97" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D97" s="15"/>
+      <c r="K97" s="12"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98" s="20"/>
+      <c r="C98" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" s="15"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99" s="20"/>
+      <c r="C99" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D99" s="15"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100" s="20"/>
+      <c r="C100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D100" s="15"/>
+      <c r="E100" s="16"/>
+      <c r="L100" s="16"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101" s="20"/>
+      <c r="C101" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D101" s="15"/>
+      <c r="K101" s="12"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102" s="20"/>
+      <c r="C102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" s="15"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103" s="20"/>
+      <c r="C103" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="15"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104" s="20"/>
+      <c r="C104" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D104" s="15"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105" s="20"/>
+      <c r="C105" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D105" s="15"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106" s="20"/>
+      <c r="C106" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D106" s="15"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107" s="20"/>
+      <c r="C107" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D107" s="15"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108" s="20"/>
+      <c r="C108" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D108" s="15"/>
+      <c r="E108" s="16"/>
+      <c r="K108" s="12"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109" s="20"/>
+      <c r="C109" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D109" s="15"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110" s="20"/>
+      <c r="C110" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D110" s="15"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111" s="20"/>
+      <c r="C111" s="22"/>
+      <c r="D111" s="15"/>
+      <c r="K111" s="12"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112" s="20"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="15"/>
+      <c r="J112" s="19"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113" s="20"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="15"/>
+      <c r="J113" s="19"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114" s="20"/>
+      <c r="C114" s="22"/>
+      <c r="D114" s="15"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115" s="20"/>
+      <c r="C115" s="22"/>
+      <c r="D115" s="15"/>
+      <c r="J115" s="19"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116" s="20"/>
+      <c r="C116" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G116" s="11"/>
+      <c r="J116" s="19"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" s="15"/>
+      <c r="E117" s="16"/>
+      <c r="K117" s="12"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>115</v>
+      </c>
+      <c r="B118" s="20"/>
+      <c r="C118" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" s="15"/>
+      <c r="E118" s="16"/>
+      <c r="K118" s="12"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119" s="20"/>
+      <c r="C119" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="15"/>
+      <c r="E119" s="16"/>
+      <c r="K119" s="12"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120" s="20"/>
+      <c r="C120" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" s="15"/>
+      <c r="E120" s="16"/>
+      <c r="K120" s="12"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E121" s="16"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122" s="20"/>
+      <c r="C122" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="22"/>
+      <c r="E122" s="16"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>120</v>
+      </c>
+      <c r="B123" s="20"/>
+      <c r="C123" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" s="22"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>121</v>
+      </c>
+      <c r="B124" s="20"/>
+      <c r="C124" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" s="22"/>
+      <c r="E124" s="16"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>122</v>
+      </c>
+      <c r="B125" s="20"/>
+      <c r="C125" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125" s="22"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>123</v>
+      </c>
+      <c r="B126" s="20"/>
+      <c r="C126" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="22"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>124</v>
+      </c>
+      <c r="B127" s="20"/>
+      <c r="C127" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" s="22"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>125</v>
+      </c>
+      <c r="B128" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D128" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" s="17"/>
+      <c r="J128" s="19"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>126</v>
+      </c>
+      <c r="B129" s="20"/>
+      <c r="C129" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="22"/>
+      <c r="E129" s="16"/>
+      <c r="F129" s="17"/>
+      <c r="K129" s="12"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>127</v>
+      </c>
+      <c r="B130" s="20"/>
+      <c r="C130" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" s="22"/>
+      <c r="F130" s="17"/>
+      <c r="J130" s="19"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>128</v>
+      </c>
+      <c r="B131" s="20"/>
+      <c r="C131" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" s="22"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="17"/>
+      <c r="K131" s="12"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>129</v>
+      </c>
+      <c r="B132" s="20"/>
+      <c r="C132" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="22"/>
+      <c r="F132" s="17"/>
+      <c r="J132" s="19"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>130</v>
+      </c>
+      <c r="B133" s="20"/>
+      <c r="C133" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="22"/>
+      <c r="F133" s="17"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="B134" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D134" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F134" s="17"/>
+      <c r="K134" s="12"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>132</v>
+      </c>
+      <c r="B135" s="20"/>
+      <c r="C135" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D135" s="22"/>
+      <c r="E135" s="16"/>
+      <c r="F135" s="17"/>
+      <c r="K135" s="12"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>133</v>
+      </c>
+      <c r="B136" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F136" s="17"/>
+      <c r="K136" s="12"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>134</v>
+      </c>
+      <c r="B137" s="20"/>
+      <c r="C137" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D137" s="21"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="17"/>
+      <c r="K137" s="12"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E139" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J139" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>87</v>
+      </c>
+      <c r="F140" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K140" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G141" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H142" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="145" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E145" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="146" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E146" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="147" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G147" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H147" s="26"/>
+    </row>
+    <row r="149" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E149" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F149" s="26"/>
+      <c r="G149" s="26"/>
+      <c r="H149" s="26"/>
+      <c r="I149" s="26"/>
+      <c r="J149" s="26"/>
+      <c r="K149" s="26"/>
+      <c r="L149" s="26"/>
+      <c r="M149" s="26"/>
+      <c r="N149" s="26"/>
+    </row>
+    <row r="150" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E150" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F150" s="26"/>
+      <c r="G150" s="26"/>
+      <c r="H150" s="26"/>
+      <c r="I150" s="26"/>
+      <c r="J150" s="26"/>
+      <c r="K150" s="26"/>
+      <c r="L150" s="26"/>
+      <c r="M150" s="26"/>
+      <c r="N150" s="26"/>
+    </row>
+    <row r="151" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E151" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F151" s="26"/>
+      <c r="G151" s="26"/>
+      <c r="H151" s="26"/>
+      <c r="I151" s="26"/>
+      <c r="J151" s="26"/>
+      <c r="K151" s="26"/>
+      <c r="L151" s="26"/>
+      <c r="M151" s="26"/>
+      <c r="N151" s="26"/>
+    </row>
+    <row r="152" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E152" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F152" s="25"/>
+      <c r="G152" s="25"/>
+      <c r="H152" s="25"/>
+      <c r="I152" s="25"/>
+      <c r="J152" s="25"/>
+      <c r="K152" s="25"/>
+      <c r="L152" s="25"/>
+      <c r="M152" s="25"/>
+      <c r="N152" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B95:B116"/>
+    <mergeCell ref="C110:C115"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="B3:B70"/>
+    <mergeCell ref="D3:D19"/>
+    <mergeCell ref="C7:C19"/>
+    <mergeCell ref="D20:D36"/>
+    <mergeCell ref="C24:C36"/>
+    <mergeCell ref="D37:D53"/>
+    <mergeCell ref="C41:C53"/>
+    <mergeCell ref="D54:D70"/>
+    <mergeCell ref="C58:C70"/>
+    <mergeCell ref="E152:N152"/>
+    <mergeCell ref="D72:D88"/>
+    <mergeCell ref="C89:C94"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="E149:N149"/>
+    <mergeCell ref="E150:N150"/>
+    <mergeCell ref="E151:N151"/>
+    <mergeCell ref="B121:B127"/>
+    <mergeCell ref="D121:D127"/>
+    <mergeCell ref="B128:B133"/>
+    <mergeCell ref="D128:D133"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="B71:B94"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91041C9-AF25-E448-A618-09FA404975FD}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <v>2013</v>
+      </c>
+      <c r="C2" s="16">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <v>106</v>
+      </c>
+      <c r="F2">
+        <v>103</v>
+      </c>
+      <c r="G2">
+        <v>118</v>
+      </c>
+      <c r="H2">
+        <v>109</v>
+      </c>
+      <c r="I2">
+        <v>128</v>
+      </c>
+      <c r="J2">
+        <v>117</v>
+      </c>
+      <c r="K2">
+        <v>125</v>
+      </c>
+      <c r="L2">
+        <v>120</v>
+      </c>
+      <c r="M2">
+        <v>107</v>
+      </c>
+      <c r="N2">
+        <v>120</v>
+      </c>
+      <c r="O2" s="16">
+        <f>AVERAGE(E2:N2)</f>
+        <v>115.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2014</v>
+      </c>
+      <c r="C3" s="16">
+        <v>121</v>
+      </c>
+      <c r="E3">
+        <v>95</v>
+      </c>
+      <c r="F3">
+        <v>115</v>
+      </c>
+      <c r="G3">
+        <v>114</v>
+      </c>
+      <c r="H3">
+        <v>87</v>
+      </c>
+      <c r="I3">
+        <v>117</v>
+      </c>
+      <c r="J3">
+        <v>122</v>
+      </c>
+      <c r="K3">
+        <v>76</v>
+      </c>
+      <c r="L3">
+        <v>102</v>
+      </c>
+      <c r="M3">
+        <v>102</v>
+      </c>
+      <c r="N3">
+        <v>117</v>
+      </c>
+      <c r="O3" s="16">
+        <f>AVERAGE(E3:N3)</f>
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2015</v>
+      </c>
+      <c r="C4" s="16">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>49</v>
+      </c>
+      <c r="F4">
+        <v>53</v>
+      </c>
+      <c r="G4">
+        <v>49</v>
+      </c>
+      <c r="H4">
+        <v>58</v>
+      </c>
+      <c r="I4">
+        <v>47</v>
+      </c>
+      <c r="J4">
+        <v>48</v>
+      </c>
+      <c r="K4">
+        <v>58</v>
+      </c>
+      <c r="L4">
+        <v>56</v>
+      </c>
+      <c r="M4">
+        <v>48</v>
+      </c>
+      <c r="N4">
+        <v>46</v>
+      </c>
+      <c r="O4" s="16">
+        <f t="shared" ref="O4:O8" si="0">AVERAGE(E4:N4)</f>
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C5" s="16"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
+        <v>2013</v>
+      </c>
+      <c r="C6" s="16">
+        <v>98</v>
+      </c>
+      <c r="E6">
+        <v>82</v>
+      </c>
+      <c r="F6">
+        <v>86</v>
+      </c>
+      <c r="G6">
+        <v>79</v>
+      </c>
+      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="I6">
+        <v>87</v>
+      </c>
+      <c r="J6">
+        <v>85</v>
+      </c>
+      <c r="K6">
+        <v>94</v>
+      </c>
+      <c r="L6">
+        <v>88</v>
+      </c>
+      <c r="M6">
+        <v>83</v>
+      </c>
+      <c r="N6">
+        <v>82</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="0"/>
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2014</v>
+      </c>
+      <c r="C7" s="16">
+        <v>124</v>
+      </c>
+      <c r="E7">
+        <v>120</v>
+      </c>
+      <c r="F7">
+        <v>113</v>
+      </c>
+      <c r="G7">
+        <v>126</v>
+      </c>
+      <c r="H7">
+        <v>124</v>
+      </c>
+      <c r="I7">
+        <v>124</v>
+      </c>
+      <c r="J7">
+        <v>125</v>
+      </c>
+      <c r="K7">
+        <v>131</v>
+      </c>
+      <c r="L7">
+        <v>128</v>
+      </c>
+      <c r="M7">
+        <v>139</v>
+      </c>
+      <c r="N7">
+        <v>119</v>
+      </c>
+      <c r="O7" s="16">
+        <f t="shared" si="0"/>
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>2015</v>
+      </c>
+      <c r="C8" s="16">
+        <v>95</v>
+      </c>
+      <c r="E8">
+        <v>93</v>
+      </c>
+      <c r="F8">
+        <v>91</v>
+      </c>
+      <c r="G8">
+        <v>93</v>
+      </c>
+      <c r="H8">
+        <v>91</v>
+      </c>
+      <c r="I8">
+        <v>81</v>
+      </c>
+      <c r="J8">
+        <v>94</v>
+      </c>
+      <c r="K8">
+        <v>138</v>
+      </c>
+      <c r="L8">
+        <v>91</v>
+      </c>
+      <c r="M8">
+        <v>88</v>
+      </c>
+      <c r="N8">
+        <v>98</v>
+      </c>
+      <c r="O8" s="16">
+        <f t="shared" si="0"/>
+        <v>95.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>